<commit_message>
Added number of cyclist
</commit_message>
<xml_diff>
--- a/results_amsterdam.xlsx
+++ b/results_amsterdam.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Postcode</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Area (km2)</t>
+  </si>
+  <si>
+    <t>Number of cyclists</t>
   </si>
   <si>
     <t>Beardwood approx</t>
@@ -527,13 +530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,13 +573,16 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>18819</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1415</v>
@@ -585,39 +591,42 @@
         <v>0.9747746508979329</v>
       </c>
       <c r="E2">
+        <v>48</v>
+      </c>
+      <c r="F2">
         <v>4.304749516699069</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2">
         <v>12.33556568715768</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>10.69527433728977</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4.526052084312471</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>12.36237187443116</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>10.69527433728977</v>
-      </c>
-      <c r="L2">
-        <v>4.526052084312471</v>
       </c>
       <c r="M2">
         <v>4.526052084312471</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>4.526052084312471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>17636</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>1183</v>
@@ -626,39 +635,42 @@
         <v>1.15988624295366</v>
       </c>
       <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
         <v>4.293560863666535</v>
       </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
         <v>13.89626777715002</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>9.121014790834892</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>6.674632285636681</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>11.62743798770239</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9.121014790834892</v>
-      </c>
-      <c r="L3">
-        <v>6.674632285636681</v>
       </c>
       <c r="M3">
         <v>6.674632285636681</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>6.674632285636681</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>29494</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -667,25 +679,25 @@
         <v>0.8040978474489774</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>0.1469897327243473</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
         <v>11.11427440205262</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2.570609958334908</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>4.795006910945239</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>6.221823986685857</v>
-      </c>
-      <c r="K4">
-        <v>2.570609958334908</v>
       </c>
       <c r="L4">
         <v>2.570609958334908</v>
@@ -693,13 +705,16 @@
       <c r="M4">
         <v>2.570609958334908</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>2.570609958334908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>12483</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>2124</v>
@@ -708,39 +723,42 @@
         <v>1.302557399618164</v>
       </c>
       <c r="E5">
+        <v>71</v>
+      </c>
+      <c r="F5">
         <v>6.096677802549377</v>
       </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
         <v>13.27895986076727</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>9.11734413727239</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>8.618551116685584</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>11.81700612548649</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>9.11734413727239</v>
-      </c>
-      <c r="L5">
-        <v>8.618551116685584</v>
       </c>
       <c r="M5">
         <v>8.618551116685584</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>8.618551116685584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>29493</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -749,25 +767,25 @@
         <v>0.9439289772783664</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>0.1126126586789276</v>
       </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
         <v>14.90689833360443</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.297044294805528</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>9.358603262886472</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>7.090886068044187</v>
-      </c>
-      <c r="K6">
-        <v>1.297044294805528</v>
       </c>
       <c r="L6">
         <v>1.297044294805528</v>
@@ -775,13 +793,16 @@
       <c r="M6">
         <v>1.297044294805528</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>1.297044294805528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>29498</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -790,25 +811,25 @@
         <v>0.9764210987849307</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>0.1145344488284531</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
         <v>15.12005626992834</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.7765025423042309</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>9.785603378299069</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6.195692125735773</v>
-      </c>
-      <c r="K7">
-        <v>0.7765025423042309</v>
       </c>
       <c r="L7">
         <v>0.7765025423042309</v>
@@ -816,13 +837,16 @@
       <c r="M7">
         <v>0.7765025423042309</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>0.7765025423042309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>7569</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>3093</v>
@@ -831,25 +855,25 @@
         <v>1.357798101796566</v>
       </c>
       <c r="E8">
+        <v>104</v>
+      </c>
+      <c r="F8">
         <v>7.511473012205087</v>
       </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
         <v>16.83306158457055</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>8.478995169314338</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>13.04791306291787</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>10.79395140720058</v>
-      </c>
-      <c r="K8">
-        <v>8.478995169314338</v>
       </c>
       <c r="L8">
         <v>8.478995169314338</v>
@@ -857,13 +881,16 @@
       <c r="M8">
         <v>8.478995169314338</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>8.478995169314338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>3533</v>
@@ -872,39 +899,42 @@
         <v>0.6090594367005497</v>
       </c>
       <c r="E9">
+        <v>118</v>
+      </c>
+      <c r="F9">
         <v>5.376742148408964</v>
       </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9">
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9">
         <v>12.82961608133535</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>9.941487352339093</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>9.536104778283807</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>9.46686907592181</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>9.941487352339093</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9.536104778283807</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>9.46686907592181</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>20234</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>3040</v>
@@ -913,39 +943,42 @@
         <v>0.5742311438456202</v>
       </c>
       <c r="E10">
+        <v>102</v>
+      </c>
+      <c r="F10">
         <v>4.842813182928229</v>
       </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10">
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10">
         <v>10.95293194149148</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>10.59693735044435</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>8.536498650890225</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>10.27683206734445</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>10.59693735044435</v>
-      </c>
-      <c r="L10">
-        <v>8.536498650890225</v>
       </c>
       <c r="M10">
         <v>8.536498650890225</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>8.536498650890225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>15815</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>1821</v>
@@ -954,39 +987,42 @@
         <v>0.4282195538587712</v>
       </c>
       <c r="E11">
+        <v>61</v>
+      </c>
+      <c r="F11">
         <v>3.236724780835308</v>
       </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11">
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11">
         <v>8.302938531212446</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>10.39026508868898</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>6.000409011035804</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>10.35262469848881</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>8.302938531212446</v>
-      </c>
-      <c r="L11">
-        <v>6.000409011035804</v>
       </c>
       <c r="M11">
         <v>6.000409011035804</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>6.000409011035804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>29497</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -995,25 +1031,25 @@
         <v>1.055751599013353</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>0.1190963431131912</v>
       </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12">
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12">
         <v>12.76139714782053</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1.202818067590609</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>9.389474088558416</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>3.371283090002177</v>
-      </c>
-      <c r="K12">
-        <v>1.202818067590609</v>
       </c>
       <c r="L12">
         <v>1.202818067590609</v>
@@ -1021,13 +1057,16 @@
       <c r="M12">
         <v>1.202818067590609</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>1.202818067590609</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>29496</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1036,39 +1075,42 @@
         <v>1.394134866168833</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>0.1368579237068646</v>
       </c>
-      <c r="F13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13">
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13">
         <v>12.61573392979467</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2.817222051060567</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>10.22957828599574</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.892894824420831</v>
-      </c>
-      <c r="K13">
-        <v>2.817222051060567</v>
       </c>
       <c r="L13">
         <v>2.817222051060567</v>
       </c>
       <c r="M13">
+        <v>2.817222051060567</v>
+      </c>
+      <c r="N13">
         <v>0.892894824420831</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>10662</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>1821</v>
@@ -1077,39 +1119,42 @@
         <v>1.751723218169205</v>
       </c>
       <c r="E14">
+        <v>61</v>
+      </c>
+      <c r="F14">
         <v>6.546441159090284</v>
       </c>
-      <c r="F14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14">
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14">
         <v>15.7836703420725</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>9.162184743894903</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>13.43861284073972</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>7.161646298044104</v>
-      </c>
-      <c r="K14">
-        <v>9.162184743894903</v>
       </c>
       <c r="L14">
         <v>9.162184743894903</v>
       </c>
       <c r="M14">
+        <v>9.162184743894903</v>
+      </c>
+      <c r="N14">
         <v>7.161646298044104</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>24413</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>2895</v>
@@ -1118,39 +1163,42 @@
         <v>1.07636630016659</v>
       </c>
       <c r="E15">
+        <v>97</v>
+      </c>
+      <c r="F15">
         <v>6.470262235006829</v>
       </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15">
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15">
         <v>10.95030496021077</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>11.87106835046616</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>10.44389244039271</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>9.308181101836952</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>10.95030496021077</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>10.44389244039271</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>9.308181101836952</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>5178</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>2391</v>
@@ -1159,25 +1207,25 @@
         <v>1.557318503676016</v>
       </c>
       <c r="E16">
+        <v>80</v>
+      </c>
+      <c r="F16">
         <v>7.072876299351764</v>
       </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16">
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16">
         <v>10.60299825384934</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>14.25147303392702</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>11.56011916503537</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>11.07920232186001</v>
-      </c>
-      <c r="K16">
-        <v>10.60299825384934</v>
       </c>
       <c r="L16">
         <v>10.60299825384934</v>
@@ -1185,13 +1233,16 @@
       <c r="M16">
         <v>10.60299825384934</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>10.60299825384934</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>29490</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1200,25 +1251,25 @@
         <v>3.220500445745016</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>0.3602797575217521</v>
       </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17">
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17">
         <v>9.801001551563072</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>22.11171259933013</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>12.49530730992685</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>21.09385274941369</v>
-      </c>
-      <c r="K17">
-        <v>9.801001551563072</v>
       </c>
       <c r="L17">
         <v>9.801001551563072</v>
@@ -1226,13 +1277,16 @@
       <c r="M17">
         <v>9.801001551563072</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>9.801001551563072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>27308</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>2182</v>
@@ -1241,39 +1295,42 @@
         <v>0.9567470628450729</v>
       </c>
       <c r="E18">
+        <v>73</v>
+      </c>
+      <c r="F18">
         <v>5.295945346206951</v>
       </c>
-      <c r="F18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18">
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18">
         <v>9.347644917516181</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>13.46170717348764</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>6.926582345141716</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>13.40606935820929</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>9.347644917516181</v>
-      </c>
-      <c r="L18">
-        <v>6.926582345141716</v>
       </c>
       <c r="M18">
         <v>6.926582345141716</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18">
+        <v>6.926582345141716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>23274</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>1139</v>
@@ -1282,39 +1339,42 @@
         <v>0.6152818792937533</v>
       </c>
       <c r="E19">
+        <v>38</v>
+      </c>
+      <c r="F19">
         <v>3.068431815031625</v>
       </c>
-      <c r="F19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19">
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19">
         <v>7.115135970268708</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>13.27905268401697</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>4.69629627445446</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>13.28463064172091</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>7.115135970268708</v>
-      </c>
-      <c r="L19">
-        <v>4.69629627445446</v>
       </c>
       <c r="M19">
         <v>4.69629627445446</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>4.69629627445446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>14607</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>1208</v>
@@ -1323,25 +1383,25 @@
         <v>3.128320564287998</v>
       </c>
       <c r="E20">
+        <v>41</v>
+      </c>
+      <c r="F20">
         <v>7.125357261932462</v>
       </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20">
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20">
         <v>7.467893234285894</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>16.48536146562533</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>11.87692886864408</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>12.47647079522626</v>
-      </c>
-      <c r="K20">
-        <v>7.467893234285894</v>
       </c>
       <c r="L20">
         <v>7.467893234285894</v>
@@ -1349,13 +1409,16 @@
       <c r="M20">
         <v>7.467893234285894</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>7.467893234285894</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>3533</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>1645</v>
@@ -1364,30 +1427,33 @@
         <v>2.849895004220496</v>
       </c>
       <c r="E21">
+        <v>55</v>
+      </c>
+      <c r="F21">
         <v>7.936242575254038</v>
       </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21">
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21">
         <v>8.779311555811063</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>18.08693168207189</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>11.76102802053738</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>16.53724399431631</v>
-      </c>
-      <c r="K21">
-        <v>8.779311555811063</v>
       </c>
       <c r="L21">
         <v>8.779311555811063</v>
       </c>
       <c r="M21">
+        <v>8.779311555811063</v>
+      </c>
+      <c r="N21">
         <v>8.779311555811063</v>
       </c>
     </row>

</xml_diff>